<commit_message>
Published state of ETDataset for deploy January 2022
</commit_message>
<xml_diff>
--- a/nodes_source_analyses/energy/energy/energy_flexibility_hv_opac_electricity.converter.xlsx
+++ b/nodes_source_analyses/energy/energy/energy_flexibility_hv_opac_electricity.converter.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="11011"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="11114"/>
   <workbookPr showInkAnnotation="0" codeName="ThisWorkbook" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mathijsbijkerk/Projects/etdataset/nodes_source_analyses/energy/energy/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/michieldenhaan/Code/etdataset/nodes_source_analyses/energy/energy/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D85A5C52-BB57-8E4C-B7F2-9DADCED80327}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{990D0E3E-EEFE-4A46-9B31-B6D4DEDEFA47}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1900" yWindow="1140" windowWidth="30240" windowHeight="16020" tabRatio="762" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="1140" windowWidth="27660" windowHeight="16020" tabRatio="762" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Cover sheet" sheetId="14" r:id="rId1"/>
@@ -60,7 +60,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="104">
   <si>
     <t>Source</t>
   </si>
@@ -83,9 +83,6 @@
     <t>Other</t>
   </si>
   <si>
-    <t>households_supplied_per_unit</t>
-  </si>
-  <si>
     <t>yes=1, no=0</t>
   </si>
   <si>
@@ -137,25 +134,13 @@
     <t>free_co2_factor</t>
   </si>
   <si>
-    <t>forecasting_error</t>
-  </si>
-  <si>
     <t>land_use_per_unit</t>
   </si>
   <si>
     <t>takes_part_in_ets</t>
   </si>
   <si>
-    <t>part_load_efficiency_penalty</t>
-  </si>
-  <si>
-    <t>part_load_operating_point</t>
-  </si>
-  <si>
     <t>electricity_output_capacity</t>
-  </si>
-  <si>
-    <t>heat_output_capacity</t>
   </si>
   <si>
     <t>initial_investment</t>
@@ -392,6 +377,15 @@
   <si>
     <t>Based on this it is assumed that both input and output are equal to 1400 MW.</t>
   </si>
+  <si>
+    <t>euro/MWh</t>
+  </si>
+  <si>
+    <t>max_consumption_price</t>
+  </si>
+  <si>
+    <t>marginal_costs</t>
+  </si>
 </sst>
 </file>
 
@@ -402,12 +396,19 @@
     <numFmt numFmtId="165" formatCode="0.000"/>
     <numFmt numFmtId="166" formatCode="0.0000"/>
   </numFmts>
-  <fonts count="28">
+  <fonts count="29">
     <font>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Lettertype hoofdtekst"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <sz val="12"/>
@@ -910,586 +911,586 @@
   </borders>
   <cellStyleXfs count="274">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="164">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="17" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="18" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="19" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="20" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="18" fillId="3" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="18" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="17" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="17" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="17" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="17" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="17" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="18" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="19" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="17" fillId="3" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="17" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="16" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="16" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="16" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="18" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="21" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="17" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="13" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="16" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="16" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="17" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="17" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="13" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="20" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="13" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="16" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="49" fontId="22" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="22" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="22" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="22" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="22" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="23" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="23" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="23" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="23" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="23" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="23" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="24" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="24" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="23" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="23" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="22" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="22" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="22" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="23" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="23" fillId="2" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="16" fillId="2" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="23" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="24" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="24" fillId="2" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="17" fillId="2" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="2" fontId="11" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="11" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="2" fontId="12" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="12" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="1" fontId="11" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="1" fontId="12" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="11" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="165" fontId="12" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="2" fontId="11" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="2" fontId="12" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="10" fontId="11" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="10" fontId="12" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center" indent="2"/>
     </xf>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="17" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="17" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="11" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="16" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="16" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="25" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="1" fontId="16" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="26" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="17" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="2" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="17" fillId="2" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="13" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="13" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="13" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="13" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="16" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="11" fillId="2" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="17" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="12" fillId="2" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="13" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="13" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="13" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="12" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="12" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="12" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="12" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="13" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="12" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="12" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="13" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="2" fontId="7" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="16" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="16" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="16" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="16" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="16" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="16" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="16" fillId="2" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="16" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="16" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="13" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="2" fontId="8" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="17" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="17" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="17" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="17" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="17" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="17" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="17" fillId="2" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="17" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="17" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="8" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="8" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="23" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="14" fontId="23" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="13" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="7" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="7" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="22" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="14" fontId="22" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="28" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="17" fontId="23" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="166" fontId="12" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="164" fontId="12" fillId="2" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="12" fillId="2" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="12" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="17" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="12" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="27" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="17" fontId="22" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="1" fontId="12" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" quotePrefix="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="164" fontId="11" fillId="2" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="11" fillId="2" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="11" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="16" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="12" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="24" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="25" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="25" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="25" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="25" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="25" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="25" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="25" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="25" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="25" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="11" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" quotePrefix="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="274">
@@ -2240,7 +2241,7 @@
     <row r="2" spans="1:4" ht="21">
       <c r="A2" s="1"/>
       <c r="B2" s="19" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C2" s="19"/>
     </row>
@@ -2252,28 +2253,28 @@
     <row r="4" spans="1:4">
       <c r="A4" s="1"/>
       <c r="B4" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C4" s="139" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
     </row>
     <row r="5" spans="1:4">
       <c r="A5" s="1"/>
       <c r="B5" s="3" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
     </row>
     <row r="6" spans="1:4">
       <c r="A6" s="1"/>
       <c r="B6" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C6" s="6" t="s">
         <v>16</v>
-      </c>
-      <c r="C6" s="6" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="7" spans="1:4">
@@ -2289,7 +2290,7 @@
     <row r="9" spans="1:4">
       <c r="A9" s="1"/>
       <c r="B9" s="49" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="C9" s="50"/>
       <c r="D9" s="66"/>
@@ -2303,10 +2304,10 @@
     <row r="11" spans="1:4">
       <c r="A11" s="1"/>
       <c r="B11" s="51" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="C11" s="53" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="D11" s="67"/>
     </row>
@@ -2314,7 +2315,7 @@
       <c r="A12" s="1"/>
       <c r="B12" s="51"/>
       <c r="C12" s="12" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="D12" s="67"/>
     </row>
@@ -2322,7 +2323,7 @@
       <c r="A13" s="1"/>
       <c r="B13" s="51"/>
       <c r="C13" s="54" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="D13" s="67"/>
     </row>
@@ -2330,7 +2331,7 @@
       <c r="A14" s="1"/>
       <c r="B14" s="51"/>
       <c r="C14" s="52" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="D14" s="67"/>
     </row>
@@ -2343,10 +2344,10 @@
     <row r="16" spans="1:4">
       <c r="A16" s="1"/>
       <c r="B16" s="51" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="C16" s="55" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="D16" s="67"/>
     </row>
@@ -2354,7 +2355,7 @@
       <c r="A17" s="1"/>
       <c r="B17" s="51"/>
       <c r="C17" s="56" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="D17" s="67"/>
     </row>
@@ -2362,7 +2363,7 @@
       <c r="A18" s="1"/>
       <c r="B18" s="51"/>
       <c r="C18" s="57" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="D18" s="67"/>
     </row>
@@ -2370,7 +2371,7 @@
       <c r="A19" s="1"/>
       <c r="B19" s="51"/>
       <c r="C19" s="58" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="D19" s="67"/>
     </row>
@@ -2378,7 +2379,7 @@
       <c r="A20" s="1"/>
       <c r="B20" s="59"/>
       <c r="C20" s="60" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="D20" s="67"/>
     </row>
@@ -2386,7 +2387,7 @@
       <c r="A21" s="1"/>
       <c r="B21" s="59"/>
       <c r="C21" s="61" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="D21" s="67"/>
     </row>
@@ -2394,14 +2395,14 @@
       <c r="A22" s="1"/>
       <c r="B22" s="59"/>
       <c r="C22" s="62" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="D22" s="67"/>
     </row>
     <row r="23" spans="1:4">
       <c r="B23" s="59"/>
       <c r="C23" s="63" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="D23" s="67"/>
     </row>
@@ -2421,10 +2422,10 @@
   <sheetPr codeName="Sheet2">
     <tabColor rgb="FFFFFF00"/>
   </sheetPr>
-  <dimension ref="B1:K39"/>
+  <dimension ref="B1:K36"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G25" sqref="G25"/>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="C29" sqref="C29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.7109375" defaultRowHeight="16" customHeight="1"/>
@@ -2449,28 +2450,28 @@
       <c r="G1" s="79"/>
     </row>
     <row r="2" spans="2:11" ht="16" customHeight="1">
-      <c r="B2" s="150" t="s">
-        <v>83</v>
-      </c>
-      <c r="C2" s="151"/>
-      <c r="D2" s="151"/>
-      <c r="E2" s="152"/>
+      <c r="B2" s="155" t="s">
+        <v>78</v>
+      </c>
+      <c r="C2" s="156"/>
+      <c r="D2" s="156"/>
+      <c r="E2" s="157"/>
       <c r="F2" s="79"/>
       <c r="G2" s="79"/>
     </row>
     <row r="3" spans="2:11" ht="16" customHeight="1">
-      <c r="B3" s="153"/>
-      <c r="C3" s="154"/>
-      <c r="D3" s="154"/>
-      <c r="E3" s="155"/>
+      <c r="B3" s="158"/>
+      <c r="C3" s="159"/>
+      <c r="D3" s="159"/>
+      <c r="E3" s="160"/>
       <c r="F3" s="79"/>
       <c r="G3" s="79"/>
     </row>
     <row r="4" spans="2:11" ht="32" customHeight="1">
-      <c r="B4" s="156"/>
-      <c r="C4" s="157"/>
-      <c r="D4" s="157"/>
-      <c r="E4" s="158"/>
+      <c r="B4" s="161"/>
+      <c r="C4" s="162"/>
+      <c r="D4" s="162"/>
+      <c r="E4" s="163"/>
       <c r="F4" s="79"/>
       <c r="G4" s="79"/>
     </row>
@@ -2491,17 +2492,17 @@
     <row r="7" spans="2:11" s="87" customFormat="1" ht="16" customHeight="1">
       <c r="B7" s="83"/>
       <c r="C7" s="84" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D7" s="85" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E7" s="84" t="s">
         <v>5</v>
       </c>
       <c r="F7" s="84"/>
       <c r="G7" s="84" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="H7" s="84"/>
       <c r="I7" s="84" t="s">
@@ -2523,7 +2524,7 @@
     <row r="9" spans="2:11" s="87" customFormat="1" ht="16" customHeight="1" thickBot="1">
       <c r="B9" s="88"/>
       <c r="C9" s="89" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="D9" s="90"/>
       <c r="E9" s="89"/>
@@ -2536,10 +2537,10 @@
     <row r="10" spans="2:11" s="87" customFormat="1" ht="16" customHeight="1" thickBot="1">
       <c r="B10" s="88"/>
       <c r="C10" s="101" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="D10" s="105" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="E10" s="130">
         <f>'Research data'!G6</f>
@@ -2548,17 +2549,17 @@
       <c r="F10" s="103"/>
       <c r="G10" s="104"/>
       <c r="I10" s="137" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="J10" s="91"/>
     </row>
     <row r="11" spans="2:11" s="87" customFormat="1" ht="16" customHeight="1" thickBot="1">
       <c r="B11" s="88"/>
       <c r="C11" s="101" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="D11" s="105" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="E11" s="130">
         <f>'Research data'!G7</f>
@@ -2567,14 +2568,14 @@
       <c r="F11" s="103"/>
       <c r="G11" s="104"/>
       <c r="I11" s="137" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="J11" s="91"/>
     </row>
     <row r="12" spans="2:11" s="87" customFormat="1" ht="16" customHeight="1" thickBot="1">
       <c r="B12" s="88"/>
       <c r="C12" s="133" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="D12" s="105" t="s">
         <v>4</v>
@@ -2584,21 +2585,21 @@
         <v>0.8</v>
       </c>
       <c r="F12" s="103"/>
-      <c r="G12" s="159" t="s">
-        <v>97</v>
+      <c r="G12" s="150" t="s">
+        <v>92</v>
       </c>
       <c r="I12" s="137" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="J12" s="91"/>
     </row>
     <row r="13" spans="2:11" s="87" customFormat="1" ht="16" customHeight="1" thickBot="1">
       <c r="B13" s="88"/>
       <c r="C13" s="101" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="D13" s="105" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="E13" s="130">
         <f>'Research data'!G10</f>
@@ -2607,17 +2608,17 @@
       <c r="F13" s="103"/>
       <c r="G13" s="104"/>
       <c r="I13" s="137" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="J13" s="91"/>
     </row>
     <row r="14" spans="2:11" s="87" customFormat="1" ht="16" customHeight="1" thickBot="1">
       <c r="B14" s="88"/>
-      <c r="C14" s="159" t="s">
-        <v>98</v>
+      <c r="C14" s="150" t="s">
+        <v>93</v>
       </c>
       <c r="D14" s="105" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="E14" s="130">
         <f>'Research data'!G9</f>
@@ -2625,15 +2626,15 @@
       </c>
       <c r="F14" s="103"/>
       <c r="G14" s="104"/>
-      <c r="I14" s="163" t="s">
-        <v>103</v>
+      <c r="I14" s="154" t="s">
+        <v>98</v>
       </c>
       <c r="J14" s="91"/>
     </row>
     <row r="15" spans="2:11" ht="16" customHeight="1" thickBot="1">
       <c r="B15" s="92"/>
       <c r="C15" s="103" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D15" s="105" t="s">
         <v>4</v>
@@ -2645,15 +2646,15 @@
       <c r="F15" s="103"/>
       <c r="G15" s="103"/>
       <c r="I15" s="137" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="J15" s="93"/>
       <c r="K15" s="79"/>
     </row>
     <row r="16" spans="2:11" ht="16" customHeight="1" thickBot="1">
       <c r="B16" s="92"/>
-      <c r="C16" s="103" t="s">
-        <v>25</v>
+      <c r="C16" s="107" t="s">
+        <v>62</v>
       </c>
       <c r="D16" s="105" t="s">
         <v>4</v>
@@ -2664,75 +2665,59 @@
       <c r="F16" s="103"/>
       <c r="G16" s="103"/>
       <c r="I16" s="137" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="J16" s="93"/>
       <c r="K16" s="79"/>
     </row>
-    <row r="17" spans="2:11" ht="16" customHeight="1" thickBot="1">
+    <row r="17" spans="2:10" ht="16" customHeight="1">
       <c r="B17" s="92"/>
-      <c r="C17" s="107" t="s">
-        <v>67</v>
-      </c>
-      <c r="D17" s="105" t="s">
-        <v>4</v>
-      </c>
-      <c r="E17" s="106">
-        <v>0</v>
-      </c>
-      <c r="F17" s="103"/>
-      <c r="G17" s="103"/>
-      <c r="I17" s="137" t="s">
-        <v>81</v>
-      </c>
+      <c r="C17" s="94"/>
+      <c r="D17" s="95"/>
+      <c r="E17" s="96"/>
+      <c r="F17" s="79"/>
+      <c r="G17" s="79"/>
+      <c r="I17" s="79"/>
       <c r="J17" s="93"/>
-      <c r="K17" s="79"/>
-    </row>
-    <row r="18" spans="2:11" ht="16" customHeight="1" thickBot="1">
+    </row>
+    <row r="18" spans="2:10" ht="16" customHeight="1" thickBot="1">
       <c r="B18" s="92"/>
-      <c r="C18" s="103" t="s">
-        <v>7</v>
-      </c>
-      <c r="D18" s="105" t="s">
-        <v>4</v>
-      </c>
-      <c r="E18" s="106">
-        <v>0</v>
-      </c>
-      <c r="F18" s="103"/>
-      <c r="G18" s="103"/>
-      <c r="I18" s="137" t="s">
-        <v>81</v>
-      </c>
+      <c r="C18" s="89" t="s">
+        <v>56</v>
+      </c>
+      <c r="D18" s="95"/>
+      <c r="E18" s="96"/>
+      <c r="F18" s="79"/>
+      <c r="G18" s="79"/>
+      <c r="I18" s="79"/>
       <c r="J18" s="93"/>
-      <c r="K18" s="79"/>
-    </row>
-    <row r="19" spans="2:11" ht="16" customHeight="1" thickBot="1">
+    </row>
+    <row r="19" spans="2:10" ht="16" customHeight="1" thickBot="1">
       <c r="B19" s="92"/>
       <c r="C19" s="103" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D19" s="105" t="s">
-        <v>4</v>
+        <v>21</v>
       </c>
       <c r="E19" s="106">
-        <v>0</v>
+        <f>'Research data'!G14</f>
+        <v>1785000000</v>
       </c>
       <c r="F19" s="103"/>
       <c r="G19" s="103"/>
       <c r="I19" s="137" t="s">
-        <v>81</v>
+        <v>84</v>
       </c>
       <c r="J19" s="93"/>
-      <c r="K19" s="79"/>
-    </row>
-    <row r="20" spans="2:11" ht="16" customHeight="1" thickBot="1">
+    </row>
+    <row r="20" spans="2:10" ht="16" customHeight="1" thickBot="1">
       <c r="B20" s="92"/>
       <c r="C20" s="103" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D20" s="105" t="s">
-        <v>4</v>
+        <v>21</v>
       </c>
       <c r="E20" s="106">
         <v>0</v>
@@ -2740,18 +2725,17 @@
       <c r="F20" s="103"/>
       <c r="G20" s="103"/>
       <c r="I20" s="137" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="J20" s="93"/>
-      <c r="K20" s="79"/>
-    </row>
-    <row r="21" spans="2:11" ht="16" customHeight="1" thickBot="1">
+    </row>
+    <row r="21" spans="2:10" ht="16" customHeight="1" thickBot="1">
       <c r="B21" s="92"/>
       <c r="C21" s="103" t="s">
-        <v>31</v>
+        <v>8</v>
       </c>
       <c r="D21" s="105" t="s">
-        <v>44</v>
+        <v>21</v>
       </c>
       <c r="E21" s="106">
         <v>0</v>
@@ -2759,94 +2743,108 @@
       <c r="F21" s="103"/>
       <c r="G21" s="103"/>
       <c r="I21" s="137" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="J21" s="93"/>
     </row>
-    <row r="22" spans="2:11" ht="16" customHeight="1">
+    <row r="22" spans="2:10" ht="16" customHeight="1" thickBot="1">
       <c r="B22" s="92"/>
-      <c r="C22" s="94"/>
-      <c r="D22" s="95"/>
-      <c r="E22" s="96"/>
-      <c r="F22" s="79"/>
-      <c r="G22" s="79"/>
-      <c r="I22" s="79"/>
+      <c r="C22" s="103" t="s">
+        <v>29</v>
+      </c>
+      <c r="D22" s="105" t="s">
+        <v>21</v>
+      </c>
+      <c r="E22" s="106">
+        <v>0</v>
+      </c>
+      <c r="F22" s="103"/>
+      <c r="G22" s="103"/>
+      <c r="I22" s="137" t="s">
+        <v>76</v>
+      </c>
       <c r="J22" s="93"/>
     </row>
-    <row r="23" spans="2:11" ht="16" customHeight="1" thickBot="1">
+    <row r="23" spans="2:10" ht="16" customHeight="1" thickBot="1">
       <c r="B23" s="92"/>
-      <c r="C23" s="89" t="s">
-        <v>61</v>
-      </c>
-      <c r="D23" s="95"/>
-      <c r="E23" s="96"/>
-      <c r="F23" s="79"/>
-      <c r="G23" s="79"/>
-      <c r="I23" s="79"/>
+      <c r="C23" s="103" t="s">
+        <v>30</v>
+      </c>
+      <c r="D23" s="105" t="s">
+        <v>37</v>
+      </c>
+      <c r="E23" s="108">
+        <f>'Research data'!G15</f>
+        <v>19800000</v>
+      </c>
+      <c r="F23" s="103"/>
+      <c r="G23" s="103"/>
+      <c r="I23" s="137" t="s">
+        <v>84</v>
+      </c>
       <c r="J23" s="93"/>
     </row>
-    <row r="24" spans="2:11" ht="16" customHeight="1" thickBot="1">
+    <row r="24" spans="2:10" ht="16" customHeight="1" thickBot="1">
       <c r="B24" s="92"/>
       <c r="C24" s="103" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D24" s="105" t="s">
-        <v>22</v>
-      </c>
-      <c r="E24" s="106">
-        <f>'Research data'!G14</f>
-        <v>1785000000</v>
+        <v>36</v>
+      </c>
+      <c r="E24" s="102">
+        <v>0</v>
       </c>
       <c r="F24" s="103"/>
       <c r="G24" s="103"/>
       <c r="I24" s="137" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="J24" s="93"/>
     </row>
-    <row r="25" spans="2:11" ht="16" customHeight="1" thickBot="1">
+    <row r="25" spans="2:10" ht="16" customHeight="1" thickBot="1">
       <c r="B25" s="92"/>
       <c r="C25" s="103" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D25" s="105" t="s">
-        <v>22</v>
-      </c>
-      <c r="E25" s="106">
+        <v>36</v>
+      </c>
+      <c r="E25" s="109">
         <v>0</v>
       </c>
       <c r="F25" s="103"/>
       <c r="G25" s="103"/>
       <c r="I25" s="137" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="J25" s="93"/>
     </row>
-    <row r="26" spans="2:11" ht="16" customHeight="1" thickBot="1">
+    <row r="26" spans="2:10" ht="16" customHeight="1" thickBot="1">
       <c r="B26" s="92"/>
       <c r="C26" s="103" t="s">
-        <v>9</v>
+        <v>35</v>
       </c>
       <c r="D26" s="105" t="s">
-        <v>22</v>
-      </c>
-      <c r="E26" s="106">
-        <v>0</v>
+        <v>2</v>
+      </c>
+      <c r="E26" s="102">
+        <v>7.0000000000000007E-2</v>
       </c>
       <c r="F26" s="103"/>
       <c r="G26" s="103"/>
-      <c r="I26" s="137" t="s">
-        <v>81</v>
+      <c r="I26" s="149" t="s">
+        <v>91</v>
       </c>
       <c r="J26" s="93"/>
     </row>
-    <row r="27" spans="2:11" ht="16" customHeight="1" thickBot="1">
+    <row r="27" spans="2:10" ht="16" customHeight="1" thickBot="1">
       <c r="B27" s="92"/>
       <c r="C27" s="103" t="s">
-        <v>34</v>
+        <v>25</v>
       </c>
       <c r="D27" s="105" t="s">
-        <v>22</v>
+        <v>7</v>
       </c>
       <c r="E27" s="106">
         <v>0</v>
@@ -2854,90 +2852,76 @@
       <c r="F27" s="103"/>
       <c r="G27" s="103"/>
       <c r="I27" s="137" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="J27" s="93"/>
     </row>
-    <row r="28" spans="2:11" ht="16" customHeight="1" thickBot="1">
+    <row r="28" spans="2:10" ht="16" customHeight="1" thickBot="1">
       <c r="B28" s="92"/>
       <c r="C28" s="103" t="s">
-        <v>35</v>
+        <v>102</v>
       </c>
       <c r="D28" s="105" t="s">
-        <v>42</v>
-      </c>
-      <c r="E28" s="108">
-        <f>'Research data'!G15</f>
-        <v>19800000</v>
+        <v>101</v>
+      </c>
+      <c r="E28" s="106">
+        <v>4.3</v>
       </c>
       <c r="F28" s="103"/>
       <c r="G28" s="103"/>
       <c r="I28" s="137" t="s">
-        <v>89</v>
+        <v>76</v>
       </c>
       <c r="J28" s="93"/>
     </row>
-    <row r="29" spans="2:11" ht="16" customHeight="1" thickBot="1">
+    <row r="29" spans="2:10" ht="16" customHeight="1" thickBot="1">
       <c r="B29" s="92"/>
       <c r="C29" s="103" t="s">
-        <v>36</v>
+        <v>103</v>
       </c>
       <c r="D29" s="105" t="s">
-        <v>41</v>
-      </c>
-      <c r="E29" s="102">
-        <v>0</v>
+        <v>101</v>
+      </c>
+      <c r="E29" s="106">
+        <f>E28/E12</f>
+        <v>5.3749999999999991</v>
       </c>
       <c r="F29" s="103"/>
       <c r="G29" s="103"/>
       <c r="I29" s="137" t="s">
-        <v>89</v>
+        <v>76</v>
       </c>
       <c r="J29" s="93"/>
     </row>
-    <row r="30" spans="2:11" ht="16" customHeight="1" thickBot="1">
+    <row r="30" spans="2:10" ht="16" customHeight="1">
       <c r="B30" s="92"/>
-      <c r="C30" s="103" t="s">
-        <v>37</v>
-      </c>
-      <c r="D30" s="105" t="s">
-        <v>41</v>
-      </c>
-      <c r="E30" s="109">
-        <v>0</v>
-      </c>
-      <c r="F30" s="103"/>
-      <c r="G30" s="103"/>
-      <c r="I30" s="137" t="s">
-        <v>81</v>
-      </c>
+      <c r="C30" s="79"/>
+      <c r="D30" s="95"/>
+      <c r="E30" s="97"/>
+      <c r="F30" s="79"/>
+      <c r="G30" s="79"/>
+      <c r="I30" s="79"/>
       <c r="J30" s="93"/>
     </row>
-    <row r="31" spans="2:11" ht="16" customHeight="1" thickBot="1">
+    <row r="31" spans="2:10" ht="16" customHeight="1" thickBot="1">
       <c r="B31" s="92"/>
-      <c r="C31" s="103" t="s">
-        <v>40</v>
-      </c>
-      <c r="D31" s="105" t="s">
-        <v>2</v>
-      </c>
-      <c r="E31" s="102">
-        <v>7.0000000000000007E-2</v>
-      </c>
-      <c r="F31" s="103"/>
-      <c r="G31" s="103"/>
-      <c r="I31" s="149" t="s">
-        <v>96</v>
-      </c>
+      <c r="C31" s="89" t="s">
+        <v>6</v>
+      </c>
+      <c r="D31" s="95"/>
+      <c r="E31" s="97"/>
+      <c r="F31" s="79"/>
+      <c r="G31" s="79"/>
+      <c r="I31" s="79"/>
       <c r="J31" s="93"/>
     </row>
-    <row r="32" spans="2:11" ht="16" customHeight="1" thickBot="1">
+    <row r="32" spans="2:10" ht="16" customHeight="1" thickBot="1">
       <c r="B32" s="92"/>
       <c r="C32" s="103" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="D32" s="105" t="s">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="E32" s="106">
         <v>0</v>
@@ -2945,39 +2929,55 @@
       <c r="F32" s="103"/>
       <c r="G32" s="103"/>
       <c r="I32" s="137" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="J32" s="93"/>
     </row>
-    <row r="33" spans="2:10" ht="16" customHeight="1">
+    <row r="33" spans="2:10" ht="16" customHeight="1" thickBot="1">
       <c r="B33" s="92"/>
-      <c r="C33" s="79"/>
-      <c r="D33" s="95"/>
-      <c r="E33" s="97"/>
-      <c r="F33" s="79"/>
-      <c r="G33" s="79"/>
-      <c r="I33" s="79"/>
+      <c r="C33" s="103" t="s">
+        <v>33</v>
+      </c>
+      <c r="D33" s="105" t="s">
+        <v>1</v>
+      </c>
+      <c r="E33" s="108">
+        <f>'Research data'!G18</f>
+        <v>5</v>
+      </c>
+      <c r="F33" s="103"/>
+      <c r="G33" s="103"/>
+      <c r="I33" s="137" t="s">
+        <v>84</v>
+      </c>
       <c r="J33" s="93"/>
     </row>
     <row r="34" spans="2:10" ht="16" customHeight="1" thickBot="1">
       <c r="B34" s="92"/>
-      <c r="C34" s="89" t="s">
-        <v>6</v>
-      </c>
-      <c r="D34" s="95"/>
-      <c r="E34" s="97"/>
-      <c r="F34" s="79"/>
-      <c r="G34" s="79"/>
-      <c r="I34" s="79"/>
+      <c r="C34" s="103" t="s">
+        <v>34</v>
+      </c>
+      <c r="D34" s="105" t="s">
+        <v>1</v>
+      </c>
+      <c r="E34" s="106">
+        <f>'Research data'!G19</f>
+        <v>50</v>
+      </c>
+      <c r="F34" s="103"/>
+      <c r="G34" s="103"/>
+      <c r="I34" s="137" t="s">
+        <v>84</v>
+      </c>
       <c r="J34" s="93"/>
     </row>
     <row r="35" spans="2:10" ht="16" customHeight="1" thickBot="1">
       <c r="B35" s="92"/>
       <c r="C35" s="103" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="D35" s="105" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E35" s="106">
         <v>0</v>
@@ -2985,76 +2985,20 @@
       <c r="F35" s="103"/>
       <c r="G35" s="103"/>
       <c r="I35" s="137" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="J35" s="93"/>
     </row>
     <row r="36" spans="2:10" ht="16" customHeight="1" thickBot="1">
-      <c r="B36" s="92"/>
-      <c r="C36" s="103" t="s">
-        <v>38</v>
-      </c>
-      <c r="D36" s="105" t="s">
-        <v>1</v>
-      </c>
-      <c r="E36" s="108">
-        <f>'Research data'!G18</f>
-        <v>5</v>
-      </c>
-      <c r="F36" s="103"/>
-      <c r="G36" s="103"/>
-      <c r="I36" s="137" t="s">
-        <v>89</v>
-      </c>
-      <c r="J36" s="93"/>
-    </row>
-    <row r="37" spans="2:10" ht="16" customHeight="1" thickBot="1">
-      <c r="B37" s="92"/>
-      <c r="C37" s="103" t="s">
-        <v>39</v>
-      </c>
-      <c r="D37" s="105" t="s">
-        <v>1</v>
-      </c>
-      <c r="E37" s="106">
-        <f>'Research data'!G19</f>
-        <v>50</v>
-      </c>
-      <c r="F37" s="103"/>
-      <c r="G37" s="103"/>
-      <c r="I37" s="137" t="s">
-        <v>89</v>
-      </c>
-      <c r="J37" s="93"/>
-    </row>
-    <row r="38" spans="2:10" ht="16" customHeight="1" thickBot="1">
-      <c r="B38" s="92"/>
-      <c r="C38" s="103" t="s">
-        <v>24</v>
-      </c>
-      <c r="D38" s="105" t="s">
-        <v>4</v>
-      </c>
-      <c r="E38" s="106">
-        <v>0</v>
-      </c>
-      <c r="F38" s="103"/>
-      <c r="G38" s="103"/>
-      <c r="I38" s="137" t="s">
-        <v>81</v>
-      </c>
-      <c r="J38" s="93"/>
-    </row>
-    <row r="39" spans="2:10" ht="16" customHeight="1" thickBot="1">
-      <c r="B39" s="98"/>
-      <c r="C39" s="99"/>
-      <c r="D39" s="99"/>
-      <c r="E39" s="99"/>
-      <c r="F39" s="99"/>
-      <c r="G39" s="99"/>
-      <c r="H39" s="99"/>
-      <c r="I39" s="99"/>
-      <c r="J39" s="100"/>
+      <c r="B36" s="98"/>
+      <c r="C36" s="99"/>
+      <c r="D36" s="99"/>
+      <c r="E36" s="99"/>
+      <c r="F36" s="99"/>
+      <c r="G36" s="99"/>
+      <c r="H36" s="99"/>
+      <c r="I36" s="99"/>
+      <c r="J36" s="100"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -3109,21 +3053,21 @@
     <row r="3" spans="2:12" s="15" customFormat="1">
       <c r="B3" s="14"/>
       <c r="C3" s="65" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="D3" s="8"/>
       <c r="E3" s="8"/>
       <c r="F3" s="65" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G3" s="65" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="H3" s="65"/>
       <c r="I3" s="65"/>
       <c r="J3" s="35"/>
       <c r="K3" s="65" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="L3" s="72"/>
     </row>
@@ -3143,7 +3087,7 @@
     <row r="5" spans="2:12" ht="17" thickBot="1">
       <c r="B5" s="41"/>
       <c r="C5" s="21" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="D5" s="21"/>
       <c r="E5" s="21"/>
@@ -3158,12 +3102,12 @@
     <row r="6" spans="2:12" ht="17" thickBot="1">
       <c r="B6" s="41"/>
       <c r="C6" s="128" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="D6" s="44"/>
       <c r="E6" s="44"/>
       <c r="F6" s="129" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="G6" s="146">
         <v>8400</v>
@@ -3172,19 +3116,19 @@
       <c r="I6" s="45"/>
       <c r="J6" s="43"/>
       <c r="K6" s="141" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="L6" s="73"/>
     </row>
     <row r="7" spans="2:12" ht="17" thickBot="1">
       <c r="B7" s="41"/>
       <c r="C7" s="128" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="D7" s="44"/>
       <c r="E7" s="44"/>
       <c r="F7" s="129" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="G7" s="146">
         <v>0</v>
@@ -3193,14 +3137,14 @@
       <c r="I7" s="45"/>
       <c r="J7" s="43"/>
       <c r="K7" s="141" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="L7" s="73"/>
     </row>
     <row r="8" spans="2:12" ht="17" thickBot="1">
       <c r="B8" s="41"/>
       <c r="C8" s="142" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="D8" s="44"/>
       <c r="E8" s="44"/>
@@ -3212,40 +3156,40 @@
       <c r="I8" s="45"/>
       <c r="J8" s="43"/>
       <c r="K8" s="141" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="L8" s="73"/>
     </row>
     <row r="9" spans="2:12" ht="17" thickBot="1">
       <c r="B9" s="41"/>
       <c r="C9" s="128" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="D9" s="44"/>
       <c r="E9" s="44"/>
       <c r="F9" s="129" t="s">
-        <v>44</v>
-      </c>
-      <c r="G9" s="160">
+        <v>39</v>
+      </c>
+      <c r="G9" s="151">
         <v>1400</v>
       </c>
       <c r="H9" s="45"/>
       <c r="I9" s="45"/>
       <c r="J9" s="43"/>
-      <c r="K9" s="161" t="s">
-        <v>103</v>
+      <c r="K9" s="152" t="s">
+        <v>98</v>
       </c>
       <c r="L9" s="73"/>
     </row>
     <row r="10" spans="2:12" ht="17" thickBot="1">
       <c r="B10" s="41"/>
       <c r="C10" s="128" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="D10" s="44"/>
       <c r="E10" s="44"/>
       <c r="F10" s="129" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="G10" s="146">
         <v>1400</v>
@@ -3254,14 +3198,14 @@
       <c r="I10" s="45"/>
       <c r="J10" s="43"/>
       <c r="K10" s="141" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="L10" s="73"/>
     </row>
     <row r="11" spans="2:12" ht="17" thickBot="1">
       <c r="B11" s="41"/>
       <c r="C11" s="128" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="D11" s="44"/>
       <c r="E11" s="44"/>
@@ -3275,7 +3219,7 @@
       <c r="I11" s="45"/>
       <c r="J11" s="43"/>
       <c r="K11" s="141" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="L11" s="73"/>
     </row>
@@ -3295,7 +3239,7 @@
     <row r="13" spans="2:12" ht="17" thickBot="1">
       <c r="B13" s="41"/>
       <c r="C13" s="11" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="D13" s="11"/>
       <c r="E13" s="11"/>
@@ -3310,12 +3254,12 @@
     <row r="14" spans="2:12" ht="17" thickBot="1">
       <c r="B14" s="41"/>
       <c r="C14" s="128" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="D14" s="44"/>
       <c r="E14" s="44"/>
       <c r="F14" s="129" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="G14" s="146">
         <v>1785000000</v>
@@ -3324,19 +3268,19 @@
       <c r="I14" s="45"/>
       <c r="J14" s="43"/>
       <c r="K14" s="141" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="L14" s="73"/>
     </row>
     <row r="15" spans="2:12" ht="17" thickBot="1">
       <c r="B15" s="41"/>
       <c r="C15" s="142" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="D15" s="44"/>
       <c r="E15" s="44"/>
       <c r="F15" s="143" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="G15" s="146">
         <v>19800000</v>
@@ -3345,7 +3289,7 @@
       <c r="I15" s="45"/>
       <c r="J15" s="43"/>
       <c r="K15" s="141" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="L15" s="73"/>
     </row>
@@ -3380,7 +3324,7 @@
     <row r="18" spans="2:12" ht="17" thickBot="1">
       <c r="B18" s="41"/>
       <c r="C18" s="128" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="D18" s="44" t="s">
         <v>3</v>
@@ -3389,7 +3333,7 @@
         <v>0</v>
       </c>
       <c r="F18" s="143" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
       <c r="G18" s="146">
         <v>5</v>
@@ -3398,14 +3342,14 @@
       <c r="I18" s="45"/>
       <c r="J18" s="43"/>
       <c r="K18" s="141" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="L18" s="73"/>
     </row>
     <row r="19" spans="2:12" ht="17" thickBot="1">
       <c r="B19" s="41"/>
       <c r="C19" s="142" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="D19" s="44" t="s">
         <v>1</v>
@@ -3414,7 +3358,7 @@
         <v>5</v>
       </c>
       <c r="F19" s="143" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
       <c r="G19" s="146">
         <v>50</v>
@@ -3423,7 +3367,7 @@
       <c r="I19" s="45"/>
       <c r="J19" s="43"/>
       <c r="K19" s="141" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
       <c r="L19" s="73"/>
     </row>
@@ -3487,7 +3431,7 @@
     <row r="3" spans="2:11">
       <c r="B3" s="27"/>
       <c r="C3" s="28" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D3" s="28"/>
       <c r="E3" s="28"/>
@@ -3513,29 +3457,29 @@
     <row r="5" spans="2:11">
       <c r="B5" s="32"/>
       <c r="C5" s="33" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D5" s="33"/>
       <c r="E5" s="33" t="s">
         <v>0</v>
       </c>
       <c r="F5" s="33" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G5" s="33" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="H5" s="33" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="I5" s="33" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="J5" s="34" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="K5" s="33" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="7" spans="2:11">
@@ -3546,13 +3490,13 @@
     </row>
     <row r="8" spans="2:11">
       <c r="C8" s="138" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="E8" s="22" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="F8" s="138" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="G8" s="140">
         <v>43344</v>
@@ -3564,23 +3508,23 @@
         <v>43709</v>
       </c>
       <c r="J8" s="23" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
     </row>
     <row r="9" spans="2:11">
       <c r="C9" s="22" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
     </row>
     <row r="10" spans="2:11">
       <c r="C10" s="22" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="E10" s="22" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="F10" s="22" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="G10" s="127">
         <v>43336</v>
@@ -3592,7 +3536,7 @@
         <v>44144</v>
       </c>
       <c r="K10" s="22" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
     </row>
   </sheetData>
@@ -3646,20 +3590,20 @@
         <v>0</v>
       </c>
       <c r="D4" s="117" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="E4" s="117" t="s">
         <v>5</v>
       </c>
       <c r="F4" s="117" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G4" s="117"/>
       <c r="H4" s="118"/>
       <c r="I4" s="117"/>
       <c r="J4" s="117"/>
       <c r="K4" s="119" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
     </row>
     <row r="5" spans="2:11">
@@ -3676,26 +3620,26 @@
     </row>
     <row r="6" spans="2:11">
       <c r="B6" s="14"/>
-      <c r="C6" s="162" t="s">
-        <v>103</v>
-      </c>
-      <c r="D6" s="162" t="s">
-        <v>78</v>
-      </c>
-      <c r="E6" s="162">
+      <c r="C6" s="153" t="s">
+        <v>98</v>
+      </c>
+      <c r="D6" s="153" t="s">
+        <v>73</v>
+      </c>
+      <c r="E6" s="153">
         <v>1400</v>
       </c>
-      <c r="F6" s="162" t="s">
-        <v>44</v>
-      </c>
-      <c r="G6" s="162" t="s">
-        <v>104</v>
+      <c r="F6" s="153" t="s">
+        <v>39</v>
+      </c>
+      <c r="G6" s="153" t="s">
+        <v>99</v>
       </c>
       <c r="H6" s="120"/>
       <c r="I6" s="12"/>
       <c r="J6" s="12"/>
       <c r="K6" s="122" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
     </row>
     <row r="7" spans="2:11">
@@ -3704,8 +3648,8 @@
       <c r="D7" s="12"/>
       <c r="E7" s="12"/>
       <c r="F7" s="12"/>
-      <c r="G7" s="162" t="s">
-        <v>105</v>
+      <c r="G7" s="153" t="s">
+        <v>100</v>
       </c>
       <c r="H7" s="120"/>
       <c r="I7" s="12"/>

</xml_diff>